<commit_message>
addition des menus dans le programme
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -16,6 +16,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Evenement</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>Aide de thomas schwartz pour les scénario de la bataille navale</t>
+  </si>
+  <si>
+    <t>TSZ</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,13 +69,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -68,8 +113,20 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="D11:F20" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="D11:F20"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Date" dataDxfId="4"/>
+    <tableColumn id="2" name="Evenement" dataDxfId="3"/>
+    <tableColumn id="3" name="VIP" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +171,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +206,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +388,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D11:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>44245</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de règles et commencement de la grille
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>TSZ</t>
+  </si>
+  <si>
+    <t>Résolution d'un bug pour les grilles</t>
   </si>
 </sst>
 </file>
@@ -89,13 +92,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -114,12 +117,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="D11:F20" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="D11:F20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="D11:F20"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" name="Evenement" dataDxfId="3"/>
-    <tableColumn id="3" name="VIP" dataDxfId="2"/>
+    <tableColumn id="1" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" name="Evenement" dataDxfId="1"/>
+    <tableColumn id="3" name="VIP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D11:F12"/>
+  <dimension ref="D11:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +426,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="13" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>44260</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Affichage d'une grille et vérification des coordonnées
pour quitter le jeux, mettre la valeur 35 pour la coordonnée y, ceci est temporaire.
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B69C1-3D02-4149-B5A2-477F18B8AABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -37,12 +38,15 @@
   </si>
   <si>
     <t>Résolution d'un bug pour les grilles</t>
+  </si>
+  <si>
+    <t>Finalization de la grille</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,12 +121,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="D11:F20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="D11:F20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="D11:F20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="D11:F20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataDxfId="2"/>
-    <tableColumn id="2" name="Evenement" dataDxfId="1"/>
-    <tableColumn id="3" name="VIP" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Evenement" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="VIP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -390,21 +394,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D11:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D11:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,7 +419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D12" s="3">
         <v>44245</v>
       </c>
@@ -426,12 +430,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" s="3">
         <v>44260</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="3">
+        <v>44264</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de légendes et d'une option pour quitter
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B69C1-3D02-4149-B5A2-477F18B8AABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0655AC7-8404-46BE-978F-FB5F6CAD4589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8160" yWindow="4310" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Finalization de la grille</t>
+  </si>
+  <si>
+    <t>Fin de la première version</t>
   </si>
 </sst>
 </file>
@@ -395,20 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D11:F14"/>
+  <dimension ref="D11:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D12" s="3">
         <v>44245</v>
       </c>
@@ -430,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:6" ht="29" x14ac:dyDescent="0.35">
       <c r="D13" s="3">
         <v>44260</v>
       </c>
@@ -438,12 +441,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D14" s="3">
         <v>44264</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D15" s="3">
+        <v>44266</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Ajout de légendes et d'une option pour quitter"
This reverts commit 13b40f878655b3f221236648c49170aec30195e4.
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0655AC7-8404-46BE-978F-FB5F6CAD4589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B69C1-3D02-4149-B5A2-477F18B8AABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="4310" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Finalization de la grille</t>
-  </si>
-  <si>
-    <t>Fin de la première version</t>
   </si>
 </sst>
 </file>
@@ -398,20 +395,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D11:F15"/>
+  <dimension ref="D11:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D12" s="3">
         <v>44245</v>
       </c>
@@ -433,7 +430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" s="3">
         <v>44260</v>
       </c>
@@ -441,20 +438,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D14" s="3">
         <v>44264</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D15" s="3">
-        <v>44266</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Ajout de légendes et d'une option pour quitter""
This reverts commit 9267a70a63fda8ebaa3e186e1c1aad0c2fef596c.
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B69C1-3D02-4149-B5A2-477F18B8AABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0655AC7-8404-46BE-978F-FB5F6CAD4589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8160" yWindow="4310" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Finalization de la grille</t>
+  </si>
+  <si>
+    <t>Fin de la première version</t>
   </si>
 </sst>
 </file>
@@ -395,20 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D11:F14"/>
+  <dimension ref="D11:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D12" s="3">
         <v>44245</v>
       </c>
@@ -430,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:6" ht="29" x14ac:dyDescent="0.35">
       <c r="D13" s="3">
         <v>44260</v>
       </c>
@@ -438,12 +441,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.35">
       <c r="D14" s="3">
         <v>44264</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D15" s="3">
+        <v>44266</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jours du journal de bord
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0655AC7-8404-46BE-978F-FB5F6CAD4589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545F25D9-3175-4927-A773-A7B4BBCE5078}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="4310" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -401,17 +401,17 @@
   <dimension ref="D11:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="4:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D12" s="3">
         <v>44245</v>
       </c>
@@ -433,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" s="3">
         <v>44260</v>
       </c>
@@ -441,7 +441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D14" s="3">
         <v>44264</v>
       </c>
@@ -449,9 +449,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D15" s="3">
-        <v>44266</v>
+        <v>44267</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Ajout d'un système de grille externe ainsi qu'une sélection de grille aléatoire
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545F25D9-3175-4927-A773-A7B4BBCE5078}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B393F1E8-770F-48AD-8DC2-6744C836D482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Fin de la première version</t>
+  </si>
+  <si>
+    <t>Ajout d'un système de log</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D11:F15"/>
+  <dimension ref="D11:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,6 +460,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="3">
+        <v>44287</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Remplit le journal de bord et de travail
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeBord.xlsx
+++ b/Documentation/JournalDeBord.xlsx
@@ -3,24 +3,33 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B393F1E8-770F-48AD-8DC2-6744C836D482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAAAB8B-CAD1-4D83-A1E7-321807486916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -37,9 +46,6 @@
     <t>TSZ</t>
   </si>
   <si>
-    <t>Résolution d'un bug pour les grilles</t>
-  </si>
-  <si>
     <t>Finalization de la grille</t>
   </si>
   <si>
@@ -47,6 +53,18 @@
   </si>
   <si>
     <t>Ajout d'un système de log</t>
+  </si>
+  <si>
+    <t>Ajout des fichier stoquant des grilles</t>
+  </si>
+  <si>
+    <t>Ajout d'un système d'authentification</t>
+  </si>
+  <si>
+    <t>Implémentation du score</t>
+  </si>
+  <si>
+    <t>VWM</t>
   </si>
 </sst>
 </file>
@@ -401,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D11:F16"/>
+  <dimension ref="D11:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,9 +454,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D13" s="3">
-        <v>44260</v>
+        <v>44264</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
@@ -446,7 +464,7 @@
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D14" s="3">
-        <v>44264</v>
+        <v>44267</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>6</v>
@@ -454,18 +472,37 @@
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D15" s="3">
-        <v>44267</v>
+        <v>44272</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D16" s="3">
+        <v>44285</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D17" s="3">
+        <v>44287</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="3">
+    <row r="18" spans="4:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D18" s="3">
         <v>44287</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>